<commit_message>
se adiciono formatos de arfactos de analisis
</commit_message>
<xml_diff>
--- a/sprint1/FORMATO SEGUIMIENTO-SPRINTS.xlsx
+++ b/sprint1/FORMATO SEGUIMIENTO-SPRINTS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PLANEACIÓN-21082022" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>HACER</t>
   </si>
@@ -135,13 +135,32 @@
   </si>
   <si>
     <t>Requerimientos No Funcionales - RNF - Erika</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modelo conceptual </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Entidades-Atributos-Dependencias-Cardinalidad)</t>
+    </r>
+  </si>
+  <si>
+    <t>modelo conceptual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +172,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -618,14 +645,14 @@
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
@@ -679,7 +706,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -687,7 +714,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -881,7 +908,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,6 +1253,9 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
@@ -1321,7 +1351,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="12">
         <f>SUM(H3:H14)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -1360,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,6 +1527,12 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4">

</xml_diff>